<commit_message>
se esta realizando la diapositiva de clase 6
</commit_message>
<xml_diff>
--- a/2015-2016/clases/computacion_aplicada_2/clase_4/practica_4.xlsx
+++ b/2015-2016/clases/computacion_aplicada_2/clase_4/practica_4.xlsx
@@ -479,15 +479,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="24.7109375" customWidth="1"/>
     <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="6" max="7" width="30.5703125" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" customWidth="1"/>
     <col min="8" max="8" width="51.85546875" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" customWidth="1"/>

</xml_diff>

<commit_message>
se subio las nuevas clases
</commit_message>
<xml_diff>
--- a/2015-2016/clases/computacion_aplicada_2/clase_4/practica_4.xlsx
+++ b/2015-2016/clases/computacion_aplicada_2/clase_4/practica_4.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -111,10 +112,10 @@
     <t>Busqueda de cedula a la izquierda,  y si lo encuentra mostrar el nombre, sino mostrar, Ninguno</t>
   </si>
   <si>
-    <t>Busqueda de la cedulas a la izquierda,  y si encuentran ambas, mostrar busqueda finalizada, si no, decir siga intentando.</t>
-  </si>
-  <si>
     <t>Busqueda de la cedulas a la izquierda,  y si encuentran al menos una, mostrar punto encontrado, si no encuentra ninguna, decir objetivo perdido.</t>
+  </si>
+  <si>
+    <t>Busqueda de la cedulas de la izquierda,  y si encuentran ambas, mostrar busqueda finalizada, si no, decir siga intentando.</t>
   </si>
 </sst>
 </file>
@@ -479,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,10 +512,10 @@
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="L6" s="1"/>
     </row>
@@ -525,14 +526,26 @@
       <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="F7" t="str">
+        <f>IF(IFERROR(SEARCH(G7,CONCATENATE($D$7,$D$8,$D$9,$D$10,$D$11,$D$12,$D$13,$D$14,$D$15,$D$16,$D$17,$D$18,$D$19,$D$20,$D$21,$D$22,$D$23,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29,$D$30,$D$31,$D$32,$D$33,$D$34,$D$35)),0)&gt;0,E7,"ninguno")</f>
+        <v>Nelly</v>
+      </c>
       <c r="G7">
         <v>1722455161</v>
       </c>
+      <c r="H7" t="str">
+        <f>IF(AND(IFERROR(SEARCH(I7,CONCATENATE($D$7,$D$8,$D$9,$D$10,$D$11,$D$12,$D$13,$D$14,$D$15,$D$16,$D$17,$D$18,$D$19,$D$20,$D$21,$D$22,$D$23,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29,$D$30,$D$31,$D$32,$D$33,$D$34,$D$35)),0)&gt;0,IFERROR(SEARCH(J7,CONCATENATE($D$7,$D$8,$D$9,$D$10,$D$11,$D$12,$D$13,$D$14,$D$15,$D$16,$D$17,$D$18,$D$19,$D$20,$D$21,$D$22,$D$23,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29,$D$30,$D$31,$D$32,$D$33,$D$34,$D$35)),0)&gt;0),"busqueda_finalizada","siga_intentando")</f>
+        <v>busqueda_finalizada</v>
+      </c>
       <c r="I7" s="1">
         <v>1716987076</v>
       </c>
       <c r="J7" s="1">
         <v>1724495435</v>
+      </c>
+      <c r="K7" t="str">
+        <f>IF(OR(IFERROR(SEARCH(L7,CONCATENATE($D$7,$D$8,$D$9,$D$10,$D$11,$D$12,$D$13,$D$14,$D$15,$D$16,$D$17,$D$18,$D$19,$D$20,$D$21,$D$22,$D$23,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29,$D$30,$D$31,$D$32,$D$33,$D$34,$D$35)),0)&gt;0,IFERROR(SEARCH(M7,CONCATENATE($D$7,$D$8,$D$9,$D$10,$D$11,$D$12,$D$13,$D$14,$D$15,$D$16,$D$17,$D$18,$D$19,$D$20,$D$21,$D$22,$D$23,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29,$D$30,$D$31,$D$32,$D$33,$D$34,$D$35)),0)&gt;0,IFERROR(SEARCH(N7,CONCATENATE($D$7,$D$8,$D$9,$D$10,$D$11,$D$12,$D$13,$D$14,$D$15,$D$16,$D$17,$D$18,$D$19,$D$20,$D$21,$D$22,$D$23,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29,$D$30,$D$31,$D$32,$D$33,$D$34,$D$35)),0)&gt;0),"punto encontrado","objeto perdido")</f>
+        <v>punto encontrado</v>
       </c>
       <c r="L7" s="1">
         <v>1716987078</v>
@@ -551,14 +564,26 @@
       <c r="E8" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F8" t="str">
+        <f t="shared" ref="F8:F13" si="0">IF(IFERROR(SEARCH(G8,CONCATENATE($D$7,$D$8,$D$9,$D$10,$D$11,$D$12,$D$13,$D$14,$D$15,$D$16,$D$17,$D$18,$D$19,$D$20,$D$21,$D$22,$D$23,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29,$D$30,$D$31,$D$32,$D$33,$D$34,$D$35)),0)&gt;0,E8,"ninguno")</f>
+        <v>ninguno</v>
+      </c>
       <c r="G8">
         <v>1442292827</v>
       </c>
+      <c r="H8" t="str">
+        <f t="shared" ref="H8:H13" si="1">IF(AND(IFERROR(SEARCH(I8,CONCATENATE($D$7,$D$8,$D$9,$D$10,$D$11,$D$12,$D$13,$D$14,$D$15,$D$16,$D$17,$D$18,$D$19,$D$20,$D$21,$D$22,$D$23,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29,$D$30,$D$31,$D$32,$D$33,$D$34,$D$35)),0)&gt;0,IFERROR(SEARCH(J8,CONCATENATE($D$7,$D$8,$D$9,$D$10,$D$11,$D$12,$D$13,$D$14,$D$15,$D$16,$D$17,$D$18,$D$19,$D$20,$D$21,$D$22,$D$23,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29,$D$30,$D$31,$D$32,$D$33,$D$34,$D$35)),0)&gt;0),"busqueda_finalizada","siga_intentando")</f>
+        <v>busqueda_finalizada</v>
+      </c>
       <c r="I8" s="1">
         <v>1720546919</v>
       </c>
       <c r="J8" s="1">
         <v>1718048233</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" ref="K8:K21" si="2">IF(OR(IFERROR(SEARCH(L8,CONCATENATE($D$7,$D$8,$D$9,$D$10,$D$11,$D$12,$D$13,$D$14,$D$15,$D$16,$D$17,$D$18,$D$19,$D$20,$D$21,$D$22,$D$23,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29,$D$30,$D$31,$D$32,$D$33,$D$34,$D$35)),0)&gt;0,IFERROR(SEARCH(M8,CONCATENATE($D$7,$D$8,$D$9,$D$10,$D$11,$D$12,$D$13,$D$14,$D$15,$D$16,$D$17,$D$18,$D$19,$D$20,$D$21,$D$22,$D$23,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29,$D$30,$D$31,$D$32,$D$33,$D$34,$D$35)),0)&gt;0,IFERROR(SEARCH(N8,CONCATENATE($D$7,$D$8,$D$9,$D$10,$D$11,$D$12,$D$13,$D$14,$D$15,$D$16,$D$17,$D$18,$D$19,$D$20,$D$21,$D$22,$D$23,$D$24,$D$25,$D$26,$D$27,$D$28,$D$29,$D$30,$D$31,$D$32,$D$33,$D$34,$D$35)),0)&gt;0),"punto encontrado","objeto perdido")</f>
+        <v>punto encontrado</v>
       </c>
       <c r="L8" s="1">
         <v>1724495437</v>
@@ -577,14 +602,26 @@
       <c r="E9" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>Jorge</v>
+      </c>
       <c r="G9">
         <v>1722964771</v>
       </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>siga_intentando</v>
+      </c>
       <c r="I9" s="1">
         <v>1716987081</v>
       </c>
       <c r="J9" s="1">
         <v>1724108440</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="2"/>
+        <v>punto encontrado</v>
       </c>
       <c r="L9" s="1">
         <v>1722455161</v>
@@ -603,14 +640,26 @@
       <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>ninguno</v>
+      </c>
       <c r="G10">
         <v>1700965571</v>
       </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>busqueda_finalizada</v>
+      </c>
       <c r="I10" s="1">
         <v>1724495440</v>
       </c>
       <c r="J10" s="1">
         <v>1716987082</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="2"/>
+        <v>punto encontrado</v>
       </c>
       <c r="L10" s="1">
         <v>1720488307</v>
@@ -629,14 +678,26 @@
       <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>Pablo</v>
+      </c>
       <c r="G11">
         <v>1724495439</v>
       </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>siga_intentando</v>
+      </c>
       <c r="I11" s="1">
         <v>1718048238</v>
       </c>
       <c r="J11" s="1">
         <v>1724961292</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="2"/>
+        <v>punto encontrado</v>
       </c>
       <c r="L11" s="1">
         <v>1724495438</v>
@@ -655,17 +716,29 @@
       <c r="E12" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>ninguno</v>
+      </c>
       <c r="G12" s="1">
         <v>1724108440</v>
       </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>siga_intentando</v>
+      </c>
       <c r="I12" s="1">
         <v>1725633732</v>
       </c>
       <c r="J12" s="1">
         <v>1796967022</v>
       </c>
+      <c r="K12" t="str">
+        <f t="shared" si="2"/>
+        <v>punto encontrado</v>
+      </c>
       <c r="L12" s="1">
-        <v>1029040136</v>
+        <v>1029040139</v>
       </c>
       <c r="M12" s="1">
         <v>1849518076</v>
@@ -681,14 +754,26 @@
       <c r="E13" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>Lady</v>
+      </c>
       <c r="G13" s="1">
         <v>1723632011</v>
       </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>busqueda_finalizada</v>
+      </c>
       <c r="I13" s="1">
         <v>1724495416</v>
       </c>
       <c r="J13" s="1">
         <v>1724966492</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="2"/>
+        <v>punto encontrado</v>
       </c>
       <c r="L13" s="1">
         <v>1716987080</v>
@@ -707,6 +792,10 @@
       <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="K14" t="str">
+        <f t="shared" si="2"/>
+        <v>punto encontrado</v>
+      </c>
       <c r="L14" s="1">
         <v>1724495439</v>
       </c>
@@ -724,6 +813,10 @@
       <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K15" t="str">
+        <f t="shared" si="2"/>
+        <v>punto encontrado</v>
+      </c>
       <c r="L15" s="1">
         <v>1724495410</v>
       </c>
@@ -741,6 +834,10 @@
       <c r="E16" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="K16" t="str">
+        <f t="shared" si="2"/>
+        <v>punto encontrado</v>
+      </c>
       <c r="L16" s="1">
         <v>1204954410</v>
       </c>
@@ -758,6 +855,10 @@
       <c r="E17" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="K17" t="str">
+        <f t="shared" si="2"/>
+        <v>punto encontrado</v>
+      </c>
       <c r="L17" s="1">
         <v>1724495440</v>
       </c>
@@ -775,6 +876,10 @@
       <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="K18" t="str">
+        <f t="shared" si="2"/>
+        <v>objeto perdido</v>
+      </c>
       <c r="L18" s="1">
         <v>1718044536</v>
       </c>
@@ -792,6 +897,10 @@
       <c r="E19" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="K19" t="str">
+        <f t="shared" si="2"/>
+        <v>punto encontrado</v>
+      </c>
       <c r="L19" s="1">
         <v>1716987082</v>
       </c>
@@ -809,6 +918,10 @@
       <c r="E20" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="K20" t="str">
+        <f t="shared" si="2"/>
+        <v>punto encontrado</v>
+      </c>
       <c r="L20" s="1">
         <v>1724495440</v>
       </c>
@@ -825,6 +938,10 @@
       </c>
       <c r="E21" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="2"/>
+        <v>objeto perdido</v>
       </c>
       <c r="L21" s="1">
         <v>1090445136</v>

</xml_diff>